<commit_message>
Add ETL pipeline scripts and update data files
Introduced new ETL scripts (analysis.py, extract.py, load.py, transform.py) and updated Jupyter notebook to implement customer, order, weather, and region mapping data integration. Added and updated database and mapping files to support the pipeline, including improved weather API handling and region normalization.
</commit_message>
<xml_diff>
--- a/data/region_mapping.xlsx
+++ b/data/region_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://innio.sharepoint.com/teams/ITTransformation/Shared Documents/21 - Data &amp; Analytics/Data &amp; Analytics/Team Composition/Job Postings/Test Cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\innio_case_study\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A50DA372-EA44-4551-ACA9-6A6F824638B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C1455EC-8F9A-48BF-BCF1-3CC02FC42889}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0DA3B5-A0B6-4BCA-8E63-3B74CA696F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56B5E0DA-454C-4362-9CE0-A4D01AF506BC}"/>
+    <workbookView xWindow="3540" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{56B5E0DA-454C-4362-9CE0-A4D01AF506BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,10 +105,10 @@
     <t>Europe</t>
   </si>
   <si>
-    <t>Region starting 2016</t>
-  </si>
-  <si>
-    <t>Region until 2017</t>
+    <t>Region until 2016</t>
+  </si>
+  <si>
+    <t>Region after 2016</t>
   </si>
 </sst>
 </file>
@@ -485,7 +483,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +740,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D1F6BAFF18CB1440A74D07C05FCC1BB2" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc20d96ffd6cd424a9f2a2fdcc56ca44">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8ac989f9-0ede-4c4e-8f6c-7031f4c22e86" xmlns:ns3="7c1c8569-feb0-445a-ada3-4d5dda49330e" xmlns:ns4="55800d30-4044-4849-804b-cac89b3dde70" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9bfcf409b43443384bea3056a4bb42b1" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="8ac989f9-0ede-4c4e-8f6c-7031f4c22e86"/>
@@ -995,15 +1002,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1016,15 +1014,42 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7BC12D3-683D-4373-BAA1-C7C758B87BB6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1362AAC-38D0-46FA-9FFB-5B9C3AD5B830}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1362AAC-38D0-46FA-9FFB-5B9C3AD5B830}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7BC12D3-683D-4373-BAA1-C7C758B87BB6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8ac989f9-0ede-4c4e-8f6c-7031f4c22e86"/>
+    <ds:schemaRef ds:uri="7c1c8569-feb0-445a-ada3-4d5dda49330e"/>
+    <ds:schemaRef ds:uri="55800d30-4044-4849-804b-cac89b3dde70"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68C5E58-FCA7-4F02-A339-7BE135C883B2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68C5E58-FCA7-4F02-A339-7BE135C883B2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8ac989f9-0ede-4c4e-8f6c-7031f4c22e86"/>
+    <ds:schemaRef ds:uri="55800d30-4044-4849-804b-cac89b3dde70"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>